<commit_message>
Project plan diagram template in excel completed
</commit_message>
<xml_diff>
--- a/project-plan.xlsx
+++ b/project-plan.xlsx
@@ -23,6 +23,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Completion Week</t>
+  </si>
+  <si>
+    <t>Starting Week</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>PERT Diagram Key</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -42,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -50,12 +115,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -71,6 +220,804 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="16" name="Group 15"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5838825" y="695325"/>
+          <a:ext cx="12449175" cy="6915150"/>
+          <a:chOff x="5838825" y="695325"/>
+          <a:chExt cx="12449175" cy="6915150"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="4" name="Group 3"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="5838825" y="695325"/>
+            <a:ext cx="12449175" cy="6915150"/>
+            <a:chOff x="5886450" y="628650"/>
+            <a:chExt cx="10010775" cy="4752975"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="Rectangle 1"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5886450" y="628650"/>
+              <a:ext cx="10010775" cy="4752975"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7858125" y="733425"/>
+              <a:ext cx="5829300" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="38100" cmpd="sng">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="3200"/>
+                <a:t>PERT</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="3200" baseline="0"/>
+                <a:t> Diagram</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="3200"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="15" name="Group 14"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="6724650" y="3714750"/>
+            <a:ext cx="590550" cy="514350"/>
+            <a:chOff x="1771650" y="5543550"/>
+            <a:chExt cx="590550" cy="514350"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="Oval 12"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1771650" y="5543550"/>
+              <a:ext cx="590550" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1895475" y="5553075"/>
+              <a:ext cx="342900" cy="380999"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="2400">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>A</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Oval 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="2838450"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="2857500"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Oval 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="4743450"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="4762500"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Oval 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9820275" y="3724275"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="3733800"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>D</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142116</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10284</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>151525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="7"/>
+          <a:endCxn id="17" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7228716" y="3277475"/>
+          <a:ext cx="1087368" cy="512600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="4"/>
+          <a:endCxn id="19" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7019925" y="4229100"/>
+          <a:ext cx="1209675" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>427866</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381759</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="17" idx="5"/>
+          <a:endCxn id="21" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8733666" y="3277475"/>
+          <a:ext cx="1173093" cy="522125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>143750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381759</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="19" idx="6"/>
+          <a:endCxn id="21" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8820150" y="4163300"/>
+          <a:ext cx="1086609" cy="837325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +1283,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="AD47" sqref="AD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sub modulue files updated and fixed. Project Plan first basic draft completed
</commit_message>
<xml_diff>
--- a/project-plan.xlsx
+++ b/project-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>PERT Diagram Key</t>
+  </si>
+  <si>
+    <t>Statement of Work</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Publication Test</t>
+  </si>
+  <si>
+    <t>Draft Purposal</t>
+  </si>
+  <si>
+    <t>Draft Paper/Conference Paper</t>
+  </si>
+  <si>
+    <t>Primitive Prototype</t>
+  </si>
+  <si>
+    <t>Final Deliverable Tests and Features</t>
   </si>
 </sst>
 </file>
@@ -194,8 +215,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -203,6 +222,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -244,7 +269,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5838825" y="695325"/>
+          <a:off x="5876925" y="695325"/>
           <a:ext cx="12449175" cy="6915150"/>
           <a:chOff x="5838825" y="695325"/>
           <a:chExt cx="12449175" cy="6915150"/>
@@ -369,9 +394,9 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="6724650" y="3714750"/>
+            <a:off x="5934075" y="3609975"/>
             <a:ext cx="590550" cy="514350"/>
-            <a:chOff x="1771650" y="5543550"/>
+            <a:chOff x="981075" y="5438775"/>
             <a:chExt cx="590550" cy="514350"/>
           </a:xfrm>
         </xdr:grpSpPr>
@@ -382,7 +407,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1771650" y="5543550"/>
+              <a:off x="981075" y="5438775"/>
               <a:ext cx="590550" cy="514350"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
@@ -421,7 +446,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1895475" y="5553075"/>
+              <a:off x="1104900" y="5448300"/>
               <a:ext cx="342900" cy="380999"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -468,16 +493,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -486,7 +511,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8229600" y="2838450"/>
+          <a:off x="7200900" y="3609975"/>
           <a:ext cx="590550" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -522,16 +547,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -540,7 +565,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8362950" y="2857500"/>
+          <a:off x="7334250" y="3629025"/>
           <a:ext cx="342900" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -586,15 +611,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -603,7 +628,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8229600" y="4743450"/>
+          <a:off x="7896225" y="3609975"/>
           <a:ext cx="590550" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -639,16 +664,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -657,7 +682,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8362950" y="4762500"/>
+          <a:off x="8020050" y="3638550"/>
           <a:ext cx="342900" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -702,16 +727,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -720,7 +745,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9820275" y="3724275"/>
+          <a:off x="8943975" y="3600450"/>
           <a:ext cx="590550" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -756,16 +781,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -774,7 +799,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9944100" y="3733800"/>
+          <a:off x="9067800" y="3609975"/>
           <a:ext cx="342900" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -819,29 +844,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142116</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>10284</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>151525</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="24" name="Straight Arrow Connector 23"/>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="13" idx="7"/>
-          <a:endCxn id="17" idx="3"/>
+          <a:stCxn id="13" idx="6"/>
+          <a:endCxn id="17" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7228716" y="3277475"/>
-          <a:ext cx="1087368" cy="512600"/>
+        <a:xfrm>
+          <a:off x="6648450" y="3867150"/>
+          <a:ext cx="552450" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -869,29 +894,128 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="17" idx="4"/>
+          <a:endCxn id="34" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="4124325"/>
+          <a:ext cx="1819275" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 30"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="34" idx="6"/>
+          <a:endCxn id="50" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9544050" y="4114800"/>
+          <a:ext cx="762000" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="13" idx="4"/>
           <a:endCxn id="19" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7019925" y="4229100"/>
-          <a:ext cx="1209675" cy="771525"/>
+          <a:off x="7219950" y="3867150"/>
+          <a:ext cx="676275" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -920,28 +1044,27 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>427866</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19925</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381759</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>161050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="17" idx="5"/>
-          <a:endCxn id="21" idx="1"/>
+          <a:stCxn id="19" idx="6"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8733666" y="3277475"/>
-          <a:ext cx="1173093" cy="522125"/>
+          <a:off x="8486775" y="3867150"/>
+          <a:ext cx="476250" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -969,29 +1092,430 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>143750</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>381759</xdr:colOff>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Oval 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8953500" y="4524375"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="TextBox 34"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077325" y="4533900"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Oval 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8953500" y="5219700"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 40"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077325" y="5229225"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>F</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Arrow Connector 44"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="17" idx="4"/>
+          <a:endCxn id="40" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="4124325"/>
+          <a:ext cx="1819275" cy="1352550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Oval 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10010775" y="3600450"/>
+          <a:ext cx="590550" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="TextBox 50"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10134600" y="3609975"/>
+          <a:ext cx="342900" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>G</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Arrow Connector 30"/>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="19" idx="6"/>
-          <a:endCxn id="21" idx="3"/>
+          <a:stCxn id="21" idx="6"/>
+          <a:endCxn id="50" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8820150" y="4163300"/>
-          <a:ext cx="1086609" cy="837325"/>
+        <a:xfrm>
+          <a:off x="9534525" y="3857625"/>
+          <a:ext cx="476250" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1286,160 +1810,202 @@
   <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD47" sqref="AD47"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>